<commit_message>
Update SCAE_ER.xlsx Iteración2 y Prototipos del 1 al 10
</commit_message>
<xml_diff>
--- a/Desarrollo/SCAE/Gestión/SCAE_ER.xlsx
+++ b/Desarrollo/SCAE/Gestión/SCAE_ER.xlsx
@@ -5,16 +5,26 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ITERACION2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Prototipos" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Prototipo1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Prototipo 2" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Prototipo 3" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Prototipo 10" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Prototipo 8" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Prototipo 9" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Prototipo 6" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Prototipo 7" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Prototipo 5" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Prototipo 4" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ITERACION1!$B$3:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ITERACION1!$B$3:$F$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ITERACION1!$B$3:$F$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="124">
   <si>
     <t xml:space="preserve">LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -356,6 +366,48 @@
   </si>
   <si>
     <t xml:space="preserve">CU10-Reporte de asistencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo 001: Login de Usuarios (Móvil y Web)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo02:Recuperar Contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo 03: Seleccionar Curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo04: Marcar Asistencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo05:Modulo Profesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profesor06:Modulo Mi cuenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo07:Modulo Perfil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo08:Cambiar Contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo09:Sincronizar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo10:Habilitar/Deshabilitar delegado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo11:Reportar Asistencias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo12:Información del Curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo13:Mantenimiento Usuario(Estudiantes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo14: Editar Alumnos</t>
   </si>
 </sst>
 </file>
@@ -365,7 +417,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -446,6 +498,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -552,7 +610,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -673,6 +731,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -749,6 +815,1063 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>113760</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="image26.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2018880" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2256840</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="image27.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2104560" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>218520</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="image28.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2656800" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304560</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1333440"/>
+          <a:ext cx="304560" cy="304560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3123720</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>56520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="image1.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1962000" y="771120"/>
+          <a:ext cx="1752120" cy="3418920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3038040</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>37800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image3.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="4609800"/>
+          <a:ext cx="2885760" cy="4257360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3380760</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>75960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image2.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="9467640"/>
+          <a:ext cx="3228480" cy="4619520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2990520</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>104400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="image5.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="14487120"/>
+          <a:ext cx="2838240" cy="3676680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2952360</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="image4.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="18535680"/>
+          <a:ext cx="2800080" cy="4047840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2085480</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="image6.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="23231160"/>
+          <a:ext cx="1933200" cy="2990520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3590280</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>18720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="image7.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="27279360"/>
+          <a:ext cx="3438000" cy="4400280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523800</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3342960</xdr:colOff>
+      <xdr:row>223</xdr:row>
+      <xdr:rowOff>47160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="image9.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114200" y="32298840"/>
+          <a:ext cx="2819160" cy="4429080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3256920</xdr:colOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="image8.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="37185480"/>
+          <a:ext cx="3104640" cy="4952880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3114360</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>113760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="image10.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="42662160"/>
+          <a:ext cx="2962080" cy="4981320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>162000</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3428640</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="image11.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId11"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752400" y="48167640"/>
+          <a:ext cx="3266640" cy="4933800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>326</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3333240</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="image12.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="53511120"/>
+          <a:ext cx="3180960" cy="4952880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4495680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447120</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="image13.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5086080" y="742680"/>
+          <a:ext cx="5123880" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>361</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94680</xdr:colOff>
+      <xdr:row>390</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="image14.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId14"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="59178600"/>
+          <a:ext cx="6400440" cy="4609800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>392</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>94680</xdr:colOff>
+      <xdr:row>417</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="image15.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId15"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742680" y="64188720"/>
+          <a:ext cx="5542920" cy="3971520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2028240</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="image16.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="1875960" cy="3438000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>999720</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>56880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="image17.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4895640" y="695160"/>
+          <a:ext cx="4895640" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2390400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="image19.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2238120" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2247480</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="image18.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2095200" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2447280</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>75600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="image20.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2295000" cy="4114440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2104560</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="image23.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="1952280" cy="3552480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161280</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="image24.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="2466360" cy="4105080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1856880</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="image25.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152360" y="723600"/>
+          <a:ext cx="1704600" cy="3000240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -756,19 +1879,19 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.219387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1262,6 +2385,146 @@
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1280,22 +2543,22 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="109.341836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="110.55612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1921,4 +3184,3401 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F392"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="14"/>
+      <c r="B110" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+    </row>
+    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="14"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="14"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="14"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="14"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A122" s="14"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="14"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A123" s="14"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="14"/>
+    </row>
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A125" s="14"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A126" s="14"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="14"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A127" s="14"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="14"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A128" s="14"/>
+      <c r="B128" s="14"/>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
+      <c r="F128" s="14"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A129" s="14"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+      <c r="F129" s="14"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A130" s="14"/>
+      <c r="B130" s="14"/>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
+      <c r="F130" s="14"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A131" s="14"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="14"/>
+      <c r="D131" s="14"/>
+      <c r="E131" s="14"/>
+      <c r="F131" s="14"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A132" s="14"/>
+      <c r="B132" s="14"/>
+      <c r="C132" s="14"/>
+      <c r="D132" s="14"/>
+      <c r="E132" s="14"/>
+      <c r="F132" s="14"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A133" s="14"/>
+      <c r="B133" s="14"/>
+      <c r="C133" s="14"/>
+      <c r="D133" s="14"/>
+      <c r="E133" s="14"/>
+      <c r="F133" s="14"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A134" s="14"/>
+      <c r="B134" s="14"/>
+      <c r="C134" s="14"/>
+      <c r="D134" s="14"/>
+      <c r="E134" s="14"/>
+      <c r="F134" s="14"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A135" s="14"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="14"/>
+      <c r="D135" s="14"/>
+      <c r="E135" s="14"/>
+      <c r="F135" s="14"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A136" s="14"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="14"/>
+      <c r="D136" s="14"/>
+      <c r="E136" s="14"/>
+      <c r="F136" s="14"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A137" s="14"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="14"/>
+      <c r="D137" s="14"/>
+      <c r="E137" s="14"/>
+      <c r="F137" s="14"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A138" s="14"/>
+      <c r="B138" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C138" s="14"/>
+      <c r="D138" s="14"/>
+      <c r="E138" s="14"/>
+      <c r="F138" s="14"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A139" s="14"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+    </row>
+    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A140" s="14"/>
+      <c r="B140" s="14"/>
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="14"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="14"/>
+      <c r="D141" s="14"/>
+      <c r="E141" s="14"/>
+      <c r="F141" s="14"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="14"/>
+      <c r="F142" s="14"/>
+    </row>
+    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A143" s="14"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="14"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A144" s="14"/>
+      <c r="B144" s="14"/>
+      <c r="C144" s="14"/>
+      <c r="D144" s="14"/>
+      <c r="E144" s="14"/>
+      <c r="F144" s="14"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A145" s="14"/>
+      <c r="B145" s="14"/>
+      <c r="C145" s="14"/>
+      <c r="D145" s="14"/>
+      <c r="E145" s="14"/>
+      <c r="F145" s="14"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A146" s="14"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="14"/>
+      <c r="D146" s="14"/>
+      <c r="E146" s="14"/>
+      <c r="F146" s="14"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A147" s="14"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="14"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A148" s="14"/>
+      <c r="B148" s="14"/>
+      <c r="C148" s="14"/>
+      <c r="D148" s="14"/>
+      <c r="E148" s="14"/>
+      <c r="F148" s="14"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A149" s="14"/>
+      <c r="B149" s="14"/>
+      <c r="C149" s="14"/>
+      <c r="D149" s="14"/>
+      <c r="E149" s="14"/>
+      <c r="F149" s="14"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A150" s="14"/>
+      <c r="B150" s="14"/>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="14"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A151" s="14"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="14"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="14"/>
+      <c r="F151" s="14"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="14"/>
+      <c r="F152" s="14"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A153" s="14"/>
+      <c r="B153" s="14"/>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+    </row>
+    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A154" s="14"/>
+      <c r="B154" s="14"/>
+      <c r="C154" s="14"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
+      <c r="F154" s="14"/>
+    </row>
+    <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A155" s="14"/>
+      <c r="B155" s="14"/>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+      <c r="F155" s="14"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A156" s="14"/>
+      <c r="B156" s="14"/>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14"/>
+      <c r="F156" s="14"/>
+    </row>
+    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A157" s="14"/>
+      <c r="B157" s="14"/>
+      <c r="C157" s="14"/>
+      <c r="D157" s="14"/>
+      <c r="E157" s="14"/>
+      <c r="F157" s="14"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A158" s="14"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="14"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
+      <c r="F158" s="14"/>
+    </row>
+    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A159" s="14"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="14"/>
+      <c r="D159" s="14"/>
+      <c r="E159" s="14"/>
+      <c r="F159" s="14"/>
+    </row>
+    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A160" s="14"/>
+      <c r="B160" s="14"/>
+      <c r="C160" s="14"/>
+      <c r="D160" s="14"/>
+      <c r="E160" s="14"/>
+      <c r="F160" s="14"/>
+    </row>
+    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A161" s="14"/>
+      <c r="B161" s="14"/>
+      <c r="C161" s="14"/>
+      <c r="D161" s="14"/>
+      <c r="E161" s="14"/>
+      <c r="F161" s="14"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A162" s="14"/>
+      <c r="B162" s="14"/>
+      <c r="C162" s="14"/>
+      <c r="D162" s="14"/>
+      <c r="E162" s="14"/>
+      <c r="F162" s="14"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A163" s="14"/>
+      <c r="B163" s="14"/>
+      <c r="C163" s="14"/>
+      <c r="D163" s="14"/>
+      <c r="E163" s="14"/>
+      <c r="F163" s="14"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A164" s="14"/>
+      <c r="B164" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C164" s="14"/>
+      <c r="D164" s="14"/>
+      <c r="E164" s="14"/>
+      <c r="F164" s="14"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A165" s="14"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="14"/>
+      <c r="D165" s="14"/>
+      <c r="E165" s="14"/>
+      <c r="F165" s="14"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A166" s="14"/>
+      <c r="B166" s="14"/>
+      <c r="C166" s="14"/>
+      <c r="D166" s="14"/>
+      <c r="E166" s="14"/>
+      <c r="F166" s="14"/>
+    </row>
+    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A167" s="14"/>
+      <c r="B167" s="14"/>
+      <c r="C167" s="14"/>
+      <c r="D167" s="14"/>
+      <c r="E167" s="14"/>
+      <c r="F167" s="14"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A168" s="14"/>
+      <c r="B168" s="14"/>
+      <c r="C168" s="14"/>
+      <c r="D168" s="14"/>
+      <c r="E168" s="14"/>
+      <c r="F168" s="14"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A169" s="14"/>
+      <c r="B169" s="14"/>
+      <c r="C169" s="14"/>
+      <c r="D169" s="14"/>
+      <c r="E169" s="14"/>
+      <c r="F169" s="14"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="14"/>
+      <c r="B170" s="14"/>
+      <c r="C170" s="14"/>
+      <c r="D170" s="14"/>
+      <c r="E170" s="14"/>
+      <c r="F170" s="14"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A171" s="14"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="14"/>
+      <c r="D171" s="14"/>
+      <c r="E171" s="14"/>
+      <c r="F171" s="14"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A172" s="14"/>
+      <c r="B172" s="14"/>
+      <c r="C172" s="14"/>
+      <c r="D172" s="14"/>
+      <c r="E172" s="14"/>
+      <c r="F172" s="14"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A173" s="14"/>
+      <c r="B173" s="14"/>
+      <c r="C173" s="14"/>
+      <c r="D173" s="14"/>
+      <c r="E173" s="14"/>
+      <c r="F173" s="14"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A174" s="14"/>
+      <c r="B174" s="14"/>
+      <c r="C174" s="14"/>
+      <c r="D174" s="14"/>
+      <c r="E174" s="14"/>
+      <c r="F174" s="14"/>
+    </row>
+    <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="14"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="14"/>
+      <c r="D175" s="14"/>
+      <c r="E175" s="14"/>
+      <c r="F175" s="14"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A176" s="14"/>
+      <c r="B176" s="14"/>
+      <c r="C176" s="14"/>
+      <c r="D176" s="14"/>
+      <c r="E176" s="14"/>
+      <c r="F176" s="14"/>
+    </row>
+    <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A177" s="14"/>
+      <c r="B177" s="14"/>
+      <c r="C177" s="14"/>
+      <c r="D177" s="14"/>
+      <c r="E177" s="14"/>
+      <c r="F177" s="14"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A178" s="14"/>
+      <c r="B178" s="14"/>
+      <c r="C178" s="14"/>
+      <c r="D178" s="14"/>
+      <c r="E178" s="14"/>
+      <c r="F178" s="14"/>
+    </row>
+    <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A179" s="14"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="14"/>
+      <c r="D179" s="14"/>
+      <c r="E179" s="14"/>
+      <c r="F179" s="14"/>
+    </row>
+    <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A180" s="14"/>
+      <c r="B180" s="14"/>
+      <c r="C180" s="14"/>
+      <c r="D180" s="14"/>
+      <c r="E180" s="14"/>
+      <c r="F180" s="14"/>
+    </row>
+    <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A181" s="14"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="14"/>
+      <c r="D181" s="14"/>
+      <c r="E181" s="14"/>
+      <c r="F181" s="14"/>
+    </row>
+    <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A182" s="14"/>
+      <c r="B182" s="14"/>
+      <c r="C182" s="14"/>
+      <c r="D182" s="14"/>
+      <c r="E182" s="14"/>
+      <c r="F182" s="14"/>
+    </row>
+    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A183" s="14"/>
+      <c r="B183" s="14"/>
+      <c r="C183" s="14"/>
+      <c r="D183" s="14"/>
+      <c r="E183" s="14"/>
+      <c r="F183" s="14"/>
+    </row>
+    <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A184" s="14"/>
+      <c r="B184" s="14"/>
+      <c r="C184" s="14"/>
+      <c r="D184" s="14"/>
+      <c r="E184" s="14"/>
+      <c r="F184" s="14"/>
+    </row>
+    <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A185" s="14"/>
+      <c r="B185" s="14"/>
+      <c r="C185" s="14"/>
+      <c r="D185" s="14"/>
+      <c r="E185" s="14"/>
+      <c r="F185" s="14"/>
+    </row>
+    <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A186" s="14"/>
+      <c r="B186" s="14"/>
+      <c r="C186" s="14"/>
+      <c r="D186" s="14"/>
+      <c r="E186" s="14"/>
+      <c r="F186" s="14"/>
+    </row>
+    <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A187" s="14"/>
+      <c r="B187" s="14"/>
+      <c r="C187" s="14"/>
+      <c r="D187" s="14"/>
+      <c r="E187" s="14"/>
+      <c r="F187" s="14"/>
+    </row>
+    <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A188" s="14"/>
+      <c r="B188" s="14"/>
+      <c r="C188" s="14"/>
+      <c r="D188" s="14"/>
+      <c r="E188" s="14"/>
+      <c r="F188" s="14"/>
+    </row>
+    <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A189" s="14"/>
+      <c r="B189" s="14"/>
+      <c r="C189" s="14"/>
+      <c r="D189" s="14"/>
+      <c r="E189" s="14"/>
+      <c r="F189" s="14"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A190" s="14"/>
+      <c r="B190" s="14"/>
+      <c r="C190" s="14"/>
+      <c r="D190" s="14"/>
+      <c r="E190" s="14"/>
+      <c r="F190" s="14"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A191" s="14"/>
+      <c r="B191" s="14"/>
+      <c r="C191" s="14"/>
+      <c r="D191" s="14"/>
+      <c r="E191" s="14"/>
+      <c r="F191" s="14"/>
+    </row>
+    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A192" s="14"/>
+      <c r="C192" s="14"/>
+      <c r="D192" s="14"/>
+      <c r="E192" s="14"/>
+      <c r="F192" s="14"/>
+    </row>
+    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A193" s="14"/>
+      <c r="B193" s="14"/>
+      <c r="C193" s="14"/>
+      <c r="D193" s="14"/>
+      <c r="E193" s="14"/>
+      <c r="F193" s="14"/>
+    </row>
+    <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A194" s="14"/>
+      <c r="B194" s="14"/>
+      <c r="C194" s="14"/>
+      <c r="D194" s="14"/>
+      <c r="E194" s="14"/>
+      <c r="F194" s="14"/>
+    </row>
+    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A195" s="14"/>
+      <c r="B195" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C195" s="14"/>
+      <c r="D195" s="14"/>
+      <c r="E195" s="14"/>
+      <c r="F195" s="14"/>
+    </row>
+    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A196" s="14"/>
+      <c r="B196" s="14"/>
+      <c r="C196" s="14"/>
+      <c r="D196" s="14"/>
+      <c r="E196" s="14"/>
+      <c r="F196" s="14"/>
+    </row>
+    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A197" s="14"/>
+      <c r="B197" s="14"/>
+      <c r="C197" s="14"/>
+      <c r="D197" s="14"/>
+      <c r="E197" s="14"/>
+      <c r="F197" s="14"/>
+    </row>
+    <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A198" s="14"/>
+      <c r="B198" s="14"/>
+      <c r="C198" s="14"/>
+      <c r="D198" s="14"/>
+      <c r="E198" s="14"/>
+      <c r="F198" s="14"/>
+    </row>
+    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A199" s="14"/>
+      <c r="B199" s="14"/>
+      <c r="C199" s="14"/>
+      <c r="D199" s="14"/>
+      <c r="E199" s="14"/>
+      <c r="F199" s="14"/>
+    </row>
+    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A200" s="14"/>
+      <c r="B200" s="14"/>
+      <c r="C200" s="14"/>
+      <c r="D200" s="14"/>
+      <c r="E200" s="14"/>
+      <c r="F200" s="14"/>
+    </row>
+    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A201" s="14"/>
+      <c r="B201" s="14"/>
+      <c r="C201" s="14"/>
+      <c r="D201" s="14"/>
+      <c r="E201" s="14"/>
+      <c r="F201" s="14"/>
+    </row>
+    <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A202" s="14"/>
+      <c r="B202" s="14"/>
+      <c r="C202" s="14"/>
+      <c r="D202" s="14"/>
+      <c r="E202" s="14"/>
+      <c r="F202" s="14"/>
+    </row>
+    <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A203" s="14"/>
+      <c r="B203" s="14"/>
+      <c r="C203" s="14"/>
+      <c r="D203" s="14"/>
+      <c r="E203" s="14"/>
+      <c r="F203" s="14"/>
+    </row>
+    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A204" s="14"/>
+      <c r="B204" s="14"/>
+      <c r="C204" s="14"/>
+      <c r="D204" s="14"/>
+      <c r="E204" s="14"/>
+      <c r="F204" s="14"/>
+    </row>
+    <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A205" s="14"/>
+      <c r="B205" s="14"/>
+      <c r="C205" s="14"/>
+      <c r="D205" s="14"/>
+      <c r="E205" s="14"/>
+      <c r="F205" s="14"/>
+    </row>
+    <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A206" s="14"/>
+      <c r="B206" s="14"/>
+      <c r="C206" s="14"/>
+      <c r="D206" s="14"/>
+      <c r="E206" s="14"/>
+      <c r="F206" s="14"/>
+    </row>
+    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A207" s="14"/>
+      <c r="B207" s="14"/>
+      <c r="C207" s="14"/>
+      <c r="D207" s="14"/>
+      <c r="E207" s="14"/>
+      <c r="F207" s="14"/>
+    </row>
+    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A208" s="14"/>
+      <c r="B208" s="14"/>
+      <c r="C208" s="14"/>
+      <c r="D208" s="14"/>
+      <c r="E208" s="14"/>
+      <c r="F208" s="14"/>
+    </row>
+    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A209" s="14"/>
+      <c r="B209" s="14"/>
+      <c r="C209" s="14"/>
+      <c r="D209" s="14"/>
+      <c r="E209" s="14"/>
+      <c r="F209" s="14"/>
+    </row>
+    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A210" s="14"/>
+      <c r="B210" s="14"/>
+      <c r="C210" s="14"/>
+      <c r="D210" s="14"/>
+      <c r="E210" s="14"/>
+      <c r="F210" s="14"/>
+    </row>
+    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A211" s="14"/>
+      <c r="B211" s="14"/>
+      <c r="C211" s="14"/>
+      <c r="D211" s="14"/>
+      <c r="E211" s="14"/>
+      <c r="F211" s="14"/>
+    </row>
+    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A212" s="14"/>
+      <c r="B212" s="14"/>
+      <c r="C212" s="14"/>
+      <c r="D212" s="14"/>
+      <c r="E212" s="14"/>
+      <c r="F212" s="14"/>
+    </row>
+    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A213" s="14"/>
+      <c r="B213" s="14"/>
+      <c r="C213" s="14"/>
+      <c r="D213" s="14"/>
+      <c r="E213" s="14"/>
+      <c r="F213" s="14"/>
+    </row>
+    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A214" s="14"/>
+      <c r="B214" s="14"/>
+      <c r="C214" s="14"/>
+      <c r="D214" s="14"/>
+      <c r="E214" s="14"/>
+      <c r="F214" s="14"/>
+    </row>
+    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A215" s="14"/>
+      <c r="B215" s="14"/>
+      <c r="C215" s="14"/>
+      <c r="D215" s="14"/>
+      <c r="E215" s="14"/>
+      <c r="F215" s="14"/>
+    </row>
+    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A216" s="14"/>
+      <c r="B216" s="14"/>
+      <c r="C216" s="14"/>
+      <c r="D216" s="14"/>
+      <c r="E216" s="14"/>
+      <c r="F216" s="14"/>
+    </row>
+    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A217" s="14"/>
+      <c r="B217" s="14"/>
+      <c r="C217" s="14"/>
+      <c r="D217" s="14"/>
+      <c r="E217" s="14"/>
+      <c r="F217" s="14"/>
+    </row>
+    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A218" s="14"/>
+      <c r="B218" s="14"/>
+      <c r="C218" s="14"/>
+      <c r="D218" s="14"/>
+      <c r="E218" s="14"/>
+      <c r="F218" s="14"/>
+    </row>
+    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A219" s="14"/>
+      <c r="B219" s="14"/>
+      <c r="C219" s="14"/>
+      <c r="D219" s="14"/>
+      <c r="E219" s="14"/>
+      <c r="F219" s="14"/>
+    </row>
+    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A220" s="14"/>
+      <c r="C220" s="14"/>
+      <c r="D220" s="14"/>
+      <c r="E220" s="14"/>
+      <c r="F220" s="14"/>
+    </row>
+    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A221" s="14"/>
+      <c r="B221" s="14"/>
+      <c r="C221" s="14"/>
+      <c r="D221" s="14"/>
+      <c r="E221" s="14"/>
+      <c r="F221" s="14"/>
+    </row>
+    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A222" s="14"/>
+      <c r="C222" s="14"/>
+      <c r="D222" s="14"/>
+      <c r="E222" s="14"/>
+      <c r="F222" s="14"/>
+    </row>
+    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A223" s="14"/>
+      <c r="B223" s="14"/>
+      <c r="C223" s="14"/>
+      <c r="D223" s="14"/>
+      <c r="E223" s="14"/>
+      <c r="F223" s="14"/>
+    </row>
+    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A224" s="14"/>
+      <c r="B224" s="14"/>
+      <c r="C224" s="14"/>
+      <c r="D224" s="14"/>
+      <c r="E224" s="14"/>
+      <c r="F224" s="14"/>
+    </row>
+    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A225" s="14"/>
+      <c r="B225" s="14"/>
+      <c r="C225" s="14"/>
+      <c r="D225" s="14"/>
+      <c r="E225" s="14"/>
+      <c r="F225" s="14"/>
+    </row>
+    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A226" s="14"/>
+      <c r="B226" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C226" s="14"/>
+      <c r="D226" s="14"/>
+      <c r="E226" s="14"/>
+      <c r="F226" s="14"/>
+    </row>
+    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A227" s="14"/>
+      <c r="B227" s="14"/>
+      <c r="C227" s="14"/>
+      <c r="D227" s="14"/>
+      <c r="E227" s="14"/>
+      <c r="F227" s="14"/>
+    </row>
+    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A228" s="14"/>
+      <c r="B228" s="14"/>
+      <c r="C228" s="14"/>
+      <c r="D228" s="14"/>
+      <c r="E228" s="14"/>
+      <c r="F228" s="14"/>
+    </row>
+    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A229" s="14"/>
+      <c r="B229" s="14"/>
+      <c r="C229" s="14"/>
+      <c r="D229" s="14"/>
+      <c r="E229" s="14"/>
+      <c r="F229" s="14"/>
+    </row>
+    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A230" s="14"/>
+      <c r="B230" s="14"/>
+      <c r="C230" s="14"/>
+      <c r="D230" s="14"/>
+      <c r="E230" s="14"/>
+      <c r="F230" s="14"/>
+    </row>
+    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A231" s="14"/>
+      <c r="B231" s="14"/>
+      <c r="C231" s="14"/>
+      <c r="D231" s="14"/>
+      <c r="E231" s="14"/>
+      <c r="F231" s="14"/>
+    </row>
+    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A232" s="14"/>
+      <c r="B232" s="14"/>
+      <c r="C232" s="14"/>
+      <c r="D232" s="14"/>
+      <c r="E232" s="14"/>
+      <c r="F232" s="14"/>
+    </row>
+    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A233" s="14"/>
+      <c r="B233" s="14"/>
+      <c r="C233" s="14"/>
+      <c r="D233" s="14"/>
+      <c r="E233" s="14"/>
+      <c r="F233" s="14"/>
+    </row>
+    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A234" s="14"/>
+      <c r="B234" s="14"/>
+      <c r="C234" s="14"/>
+      <c r="D234" s="14"/>
+      <c r="E234" s="14"/>
+      <c r="F234" s="14"/>
+    </row>
+    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A235" s="14"/>
+      <c r="B235" s="14"/>
+      <c r="C235" s="14"/>
+      <c r="D235" s="14"/>
+      <c r="E235" s="14"/>
+      <c r="F235" s="14"/>
+    </row>
+    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A236" s="14"/>
+      <c r="B236" s="14"/>
+      <c r="C236" s="14"/>
+      <c r="D236" s="14"/>
+      <c r="E236" s="14"/>
+      <c r="F236" s="14"/>
+    </row>
+    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A237" s="14"/>
+      <c r="B237" s="14"/>
+      <c r="C237" s="14"/>
+      <c r="D237" s="14"/>
+      <c r="E237" s="14"/>
+      <c r="F237" s="14"/>
+    </row>
+    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A238" s="14"/>
+      <c r="B238" s="14"/>
+      <c r="C238" s="14"/>
+      <c r="D238" s="14"/>
+      <c r="E238" s="14"/>
+      <c r="F238" s="14"/>
+    </row>
+    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A239" s="14"/>
+      <c r="B239" s="14"/>
+      <c r="C239" s="14"/>
+      <c r="D239" s="14"/>
+      <c r="E239" s="14"/>
+      <c r="F239" s="14"/>
+    </row>
+    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A240" s="14"/>
+      <c r="B240" s="14"/>
+      <c r="C240" s="14"/>
+      <c r="D240" s="14"/>
+      <c r="E240" s="14"/>
+      <c r="F240" s="14"/>
+    </row>
+    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A241" s="14"/>
+      <c r="B241" s="14"/>
+      <c r="C241" s="14"/>
+      <c r="D241" s="14"/>
+      <c r="E241" s="14"/>
+      <c r="F241" s="14"/>
+    </row>
+    <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A242" s="14"/>
+      <c r="B242" s="14"/>
+      <c r="C242" s="14"/>
+      <c r="D242" s="14"/>
+      <c r="E242" s="14"/>
+      <c r="F242" s="14"/>
+    </row>
+    <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A243" s="14"/>
+      <c r="B243" s="14"/>
+      <c r="C243" s="14"/>
+      <c r="D243" s="14"/>
+      <c r="E243" s="14"/>
+      <c r="F243" s="14"/>
+    </row>
+    <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A244" s="14"/>
+      <c r="B244" s="14"/>
+      <c r="C244" s="14"/>
+      <c r="D244" s="14"/>
+      <c r="E244" s="14"/>
+      <c r="F244" s="14"/>
+    </row>
+    <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A245" s="14"/>
+      <c r="B245" s="14"/>
+      <c r="C245" s="14"/>
+      <c r="D245" s="14"/>
+      <c r="E245" s="14"/>
+      <c r="F245" s="14"/>
+    </row>
+    <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A246" s="14"/>
+      <c r="B246" s="14"/>
+      <c r="C246" s="14"/>
+      <c r="D246" s="14"/>
+      <c r="E246" s="14"/>
+      <c r="F246" s="14"/>
+    </row>
+    <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A247" s="14"/>
+      <c r="B247" s="14"/>
+      <c r="C247" s="14"/>
+      <c r="D247" s="14"/>
+      <c r="E247" s="14"/>
+      <c r="F247" s="14"/>
+    </row>
+    <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A248" s="14"/>
+      <c r="B248" s="14"/>
+      <c r="C248" s="14"/>
+      <c r="D248" s="14"/>
+      <c r="E248" s="14"/>
+      <c r="F248" s="14"/>
+    </row>
+    <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A249" s="14"/>
+      <c r="B249" s="14"/>
+      <c r="C249" s="14"/>
+      <c r="D249" s="14"/>
+      <c r="E249" s="14"/>
+      <c r="F249" s="14"/>
+    </row>
+    <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A250" s="14"/>
+      <c r="B250" s="14"/>
+      <c r="C250" s="14"/>
+      <c r="D250" s="14"/>
+      <c r="E250" s="14"/>
+      <c r="F250" s="14"/>
+    </row>
+    <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A251" s="14"/>
+      <c r="B251" s="14"/>
+      <c r="C251" s="14"/>
+      <c r="D251" s="14"/>
+      <c r="E251" s="14"/>
+      <c r="F251" s="14"/>
+    </row>
+    <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A252" s="14"/>
+      <c r="B252" s="14"/>
+      <c r="C252" s="14"/>
+      <c r="D252" s="14"/>
+      <c r="E252" s="14"/>
+      <c r="F252" s="14"/>
+    </row>
+    <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A253" s="14"/>
+      <c r="B253" s="14"/>
+      <c r="C253" s="14"/>
+      <c r="D253" s="14"/>
+      <c r="E253" s="14"/>
+      <c r="F253" s="14"/>
+    </row>
+    <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A254" s="14"/>
+      <c r="B254" s="14"/>
+      <c r="C254" s="14"/>
+      <c r="D254" s="14"/>
+      <c r="E254" s="14"/>
+      <c r="F254" s="14"/>
+    </row>
+    <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A255" s="14"/>
+      <c r="B255" s="14"/>
+      <c r="C255" s="14"/>
+      <c r="D255" s="14"/>
+      <c r="E255" s="14"/>
+      <c r="F255" s="14"/>
+    </row>
+    <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A256" s="14"/>
+      <c r="B256" s="14"/>
+      <c r="C256" s="14"/>
+      <c r="D256" s="14"/>
+      <c r="E256" s="14"/>
+      <c r="F256" s="14"/>
+    </row>
+    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A257" s="14"/>
+      <c r="B257" s="14"/>
+      <c r="C257" s="14"/>
+      <c r="D257" s="14"/>
+      <c r="E257" s="14"/>
+      <c r="F257" s="14"/>
+    </row>
+    <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A258" s="14"/>
+      <c r="B258" s="14"/>
+      <c r="C258" s="14"/>
+      <c r="D258" s="14"/>
+      <c r="E258" s="14"/>
+      <c r="F258" s="14"/>
+    </row>
+    <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A259" s="14"/>
+      <c r="B259" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C259" s="14"/>
+      <c r="D259" s="14"/>
+      <c r="E259" s="14"/>
+      <c r="F259" s="14"/>
+    </row>
+    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A260" s="14"/>
+      <c r="B260" s="14"/>
+      <c r="C260" s="14"/>
+      <c r="D260" s="14"/>
+      <c r="E260" s="14"/>
+      <c r="F260" s="14"/>
+    </row>
+    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A261" s="14"/>
+      <c r="B261" s="14"/>
+      <c r="C261" s="14"/>
+      <c r="D261" s="14"/>
+      <c r="E261" s="14"/>
+      <c r="F261" s="14"/>
+    </row>
+    <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A262" s="14"/>
+      <c r="B262" s="14"/>
+      <c r="C262" s="14"/>
+      <c r="D262" s="14"/>
+      <c r="E262" s="14"/>
+      <c r="F262" s="14"/>
+    </row>
+    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A263" s="14"/>
+      <c r="B263" s="14"/>
+      <c r="C263" s="14"/>
+      <c r="D263" s="14"/>
+      <c r="E263" s="14"/>
+      <c r="F263" s="14"/>
+    </row>
+    <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A264" s="14"/>
+      <c r="B264" s="14"/>
+      <c r="C264" s="14"/>
+      <c r="D264" s="14"/>
+      <c r="E264" s="14"/>
+      <c r="F264" s="14"/>
+    </row>
+    <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A265" s="14"/>
+      <c r="B265" s="14"/>
+      <c r="C265" s="14"/>
+      <c r="D265" s="14"/>
+      <c r="E265" s="14"/>
+      <c r="F265" s="14"/>
+    </row>
+    <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A266" s="14"/>
+      <c r="B266" s="14"/>
+      <c r="C266" s="14"/>
+      <c r="D266" s="14"/>
+      <c r="E266" s="14"/>
+      <c r="F266" s="14"/>
+    </row>
+    <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A267" s="14"/>
+      <c r="B267" s="14"/>
+      <c r="C267" s="14"/>
+      <c r="D267" s="14"/>
+      <c r="E267" s="14"/>
+      <c r="F267" s="14"/>
+    </row>
+    <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A268" s="14"/>
+      <c r="B268" s="14"/>
+      <c r="C268" s="14"/>
+      <c r="D268" s="14"/>
+      <c r="E268" s="14"/>
+      <c r="F268" s="14"/>
+    </row>
+    <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A269" s="14"/>
+      <c r="B269" s="14"/>
+      <c r="C269" s="14"/>
+      <c r="D269" s="14"/>
+      <c r="E269" s="14"/>
+      <c r="F269" s="14"/>
+    </row>
+    <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A270" s="14"/>
+      <c r="B270" s="14"/>
+      <c r="C270" s="14"/>
+      <c r="D270" s="14"/>
+      <c r="E270" s="14"/>
+      <c r="F270" s="14"/>
+    </row>
+    <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A271" s="14"/>
+      <c r="B271" s="14"/>
+      <c r="C271" s="14"/>
+      <c r="D271" s="14"/>
+      <c r="E271" s="14"/>
+      <c r="F271" s="14"/>
+    </row>
+    <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A272" s="14"/>
+      <c r="B272" s="14"/>
+      <c r="C272" s="14"/>
+      <c r="D272" s="14"/>
+      <c r="E272" s="14"/>
+      <c r="F272" s="14"/>
+    </row>
+    <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A273" s="14"/>
+      <c r="C273" s="14"/>
+      <c r="D273" s="14"/>
+      <c r="E273" s="14"/>
+      <c r="F273" s="14"/>
+    </row>
+    <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A274" s="14"/>
+      <c r="B274" s="14"/>
+      <c r="C274" s="14"/>
+      <c r="D274" s="14"/>
+      <c r="E274" s="14"/>
+      <c r="F274" s="14"/>
+    </row>
+    <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A275" s="14"/>
+      <c r="B275" s="14"/>
+      <c r="C275" s="14"/>
+      <c r="D275" s="14"/>
+      <c r="E275" s="14"/>
+      <c r="F275" s="14"/>
+    </row>
+    <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A276" s="14"/>
+      <c r="B276" s="14"/>
+      <c r="C276" s="14"/>
+      <c r="D276" s="14"/>
+      <c r="E276" s="14"/>
+      <c r="F276" s="14"/>
+    </row>
+    <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A277" s="14"/>
+      <c r="B277" s="14"/>
+      <c r="C277" s="14"/>
+      <c r="D277" s="14"/>
+      <c r="E277" s="14"/>
+      <c r="F277" s="14"/>
+    </row>
+    <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A278" s="14"/>
+      <c r="B278" s="14"/>
+      <c r="C278" s="14"/>
+      <c r="D278" s="14"/>
+      <c r="E278" s="14"/>
+      <c r="F278" s="14"/>
+    </row>
+    <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A279" s="14"/>
+      <c r="B279" s="14"/>
+      <c r="C279" s="14"/>
+      <c r="D279" s="14"/>
+      <c r="E279" s="14"/>
+      <c r="F279" s="14"/>
+    </row>
+    <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A280" s="14"/>
+      <c r="B280" s="14"/>
+      <c r="C280" s="14"/>
+      <c r="D280" s="14"/>
+      <c r="E280" s="14"/>
+      <c r="F280" s="14"/>
+    </row>
+    <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A281" s="14"/>
+      <c r="B281" s="14"/>
+      <c r="C281" s="14"/>
+      <c r="D281" s="14"/>
+      <c r="E281" s="14"/>
+      <c r="F281" s="14"/>
+    </row>
+    <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A282" s="14"/>
+      <c r="B282" s="14"/>
+      <c r="C282" s="14"/>
+      <c r="D282" s="14"/>
+      <c r="E282" s="14"/>
+      <c r="F282" s="14"/>
+    </row>
+    <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A283" s="14"/>
+      <c r="B283" s="14"/>
+      <c r="C283" s="14"/>
+      <c r="D283" s="14"/>
+      <c r="E283" s="14"/>
+      <c r="F283" s="14"/>
+    </row>
+    <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A284" s="14"/>
+      <c r="B284" s="14"/>
+      <c r="C284" s="14"/>
+      <c r="D284" s="14"/>
+      <c r="E284" s="14"/>
+      <c r="F284" s="14"/>
+    </row>
+    <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A285" s="14"/>
+      <c r="B285" s="14"/>
+      <c r="C285" s="14"/>
+      <c r="D285" s="14"/>
+      <c r="E285" s="14"/>
+      <c r="F285" s="14"/>
+    </row>
+    <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A286" s="14"/>
+      <c r="B286" s="14"/>
+      <c r="C286" s="14"/>
+      <c r="D286" s="14"/>
+      <c r="E286" s="14"/>
+      <c r="F286" s="14"/>
+    </row>
+    <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A287" s="14"/>
+      <c r="B287" s="14"/>
+      <c r="C287" s="14"/>
+      <c r="D287" s="14"/>
+      <c r="E287" s="14"/>
+      <c r="F287" s="14"/>
+    </row>
+    <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A288" s="14"/>
+      <c r="B288" s="14"/>
+      <c r="C288" s="14"/>
+      <c r="D288" s="14"/>
+      <c r="E288" s="14"/>
+      <c r="F288" s="14"/>
+    </row>
+    <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A289" s="14"/>
+      <c r="B289" s="14"/>
+      <c r="C289" s="14"/>
+      <c r="D289" s="14"/>
+      <c r="E289" s="14"/>
+      <c r="F289" s="14"/>
+    </row>
+    <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A290" s="14"/>
+      <c r="B290" s="14"/>
+      <c r="C290" s="14"/>
+      <c r="D290" s="14"/>
+      <c r="E290" s="14"/>
+      <c r="F290" s="14"/>
+    </row>
+    <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A291" s="14"/>
+      <c r="B291" s="14"/>
+      <c r="C291" s="14"/>
+      <c r="D291" s="14"/>
+      <c r="E291" s="14"/>
+      <c r="F291" s="14"/>
+    </row>
+    <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A292" s="14"/>
+      <c r="B292" s="14"/>
+      <c r="C292" s="14"/>
+      <c r="D292" s="14"/>
+      <c r="E292" s="14"/>
+      <c r="F292" s="14"/>
+    </row>
+    <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A293" s="14"/>
+      <c r="B293" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C293" s="14"/>
+      <c r="D293" s="14"/>
+      <c r="E293" s="14"/>
+      <c r="F293" s="14"/>
+    </row>
+    <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A294" s="14"/>
+      <c r="B294" s="14"/>
+      <c r="C294" s="14"/>
+      <c r="D294" s="14"/>
+      <c r="E294" s="14"/>
+      <c r="F294" s="14"/>
+    </row>
+    <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A295" s="14"/>
+      <c r="B295" s="14"/>
+      <c r="C295" s="14"/>
+      <c r="D295" s="14"/>
+      <c r="E295" s="14"/>
+      <c r="F295" s="14"/>
+    </row>
+    <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A296" s="14"/>
+      <c r="B296" s="14"/>
+      <c r="C296" s="14"/>
+      <c r="D296" s="14"/>
+      <c r="E296" s="14"/>
+      <c r="F296" s="14"/>
+    </row>
+    <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A297" s="14"/>
+      <c r="B297" s="14"/>
+      <c r="C297" s="14"/>
+      <c r="D297" s="14"/>
+      <c r="E297" s="14"/>
+      <c r="F297" s="14"/>
+    </row>
+    <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A298" s="14"/>
+      <c r="B298" s="14"/>
+      <c r="C298" s="14"/>
+      <c r="D298" s="14"/>
+      <c r="E298" s="14"/>
+      <c r="F298" s="14"/>
+    </row>
+    <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A299" s="14"/>
+      <c r="B299" s="14"/>
+      <c r="C299" s="14"/>
+      <c r="D299" s="14"/>
+      <c r="E299" s="14"/>
+      <c r="F299" s="14"/>
+    </row>
+    <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A300" s="14"/>
+      <c r="B300" s="14"/>
+      <c r="C300" s="14"/>
+      <c r="D300" s="14"/>
+      <c r="E300" s="14"/>
+      <c r="F300" s="14"/>
+    </row>
+    <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A301" s="14"/>
+      <c r="B301" s="14"/>
+      <c r="C301" s="14"/>
+      <c r="D301" s="14"/>
+      <c r="E301" s="14"/>
+      <c r="F301" s="14"/>
+    </row>
+    <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A302" s="14"/>
+      <c r="B302" s="14"/>
+      <c r="C302" s="14"/>
+      <c r="D302" s="14"/>
+      <c r="E302" s="14"/>
+      <c r="F302" s="14"/>
+    </row>
+    <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A303" s="14"/>
+      <c r="B303" s="14"/>
+      <c r="C303" s="14"/>
+      <c r="D303" s="14"/>
+      <c r="E303" s="14"/>
+      <c r="F303" s="14"/>
+    </row>
+    <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A304" s="14"/>
+      <c r="B304" s="14"/>
+      <c r="C304" s="14"/>
+      <c r="D304" s="14"/>
+      <c r="E304" s="14"/>
+      <c r="F304" s="14"/>
+    </row>
+    <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A305" s="14"/>
+      <c r="B305" s="14"/>
+      <c r="C305" s="14"/>
+      <c r="D305" s="14"/>
+      <c r="E305" s="14"/>
+      <c r="F305" s="14"/>
+    </row>
+    <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A306" s="14"/>
+      <c r="B306" s="14"/>
+      <c r="C306" s="14"/>
+      <c r="D306" s="14"/>
+      <c r="E306" s="14"/>
+      <c r="F306" s="14"/>
+    </row>
+    <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A307" s="14"/>
+      <c r="B307" s="14"/>
+      <c r="C307" s="14"/>
+      <c r="D307" s="14"/>
+      <c r="E307" s="14"/>
+      <c r="F307" s="14"/>
+    </row>
+    <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A308" s="14"/>
+      <c r="B308" s="14"/>
+      <c r="C308" s="14"/>
+      <c r="D308" s="14"/>
+      <c r="E308" s="14"/>
+      <c r="F308" s="14"/>
+    </row>
+    <row r="309" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A309" s="14"/>
+      <c r="B309" s="14"/>
+      <c r="C309" s="14"/>
+      <c r="D309" s="14"/>
+      <c r="E309" s="14"/>
+      <c r="F309" s="14"/>
+    </row>
+    <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A310" s="14"/>
+      <c r="B310" s="14"/>
+      <c r="C310" s="14"/>
+      <c r="D310" s="14"/>
+      <c r="E310" s="14"/>
+      <c r="F310" s="14"/>
+    </row>
+    <row r="311" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A311" s="14"/>
+      <c r="B311" s="14"/>
+      <c r="C311" s="14"/>
+      <c r="D311" s="14"/>
+      <c r="E311" s="14"/>
+      <c r="F311" s="14"/>
+    </row>
+    <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A312" s="14"/>
+      <c r="B312" s="14"/>
+      <c r="C312" s="14"/>
+      <c r="D312" s="14"/>
+      <c r="E312" s="14"/>
+      <c r="F312" s="14"/>
+    </row>
+    <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A313" s="14"/>
+      <c r="B313" s="14"/>
+      <c r="C313" s="14"/>
+      <c r="D313" s="14"/>
+      <c r="E313" s="14"/>
+      <c r="F313" s="14"/>
+    </row>
+    <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A314" s="14"/>
+      <c r="B314" s="14"/>
+      <c r="C314" s="14"/>
+      <c r="D314" s="14"/>
+      <c r="E314" s="14"/>
+      <c r="F314" s="14"/>
+    </row>
+    <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A315" s="14"/>
+      <c r="B315" s="14"/>
+      <c r="C315" s="14"/>
+      <c r="D315" s="14"/>
+      <c r="E315" s="14"/>
+      <c r="F315" s="14"/>
+    </row>
+    <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A316" s="14"/>
+      <c r="B316" s="14"/>
+      <c r="C316" s="14"/>
+      <c r="D316" s="14"/>
+      <c r="E316" s="14"/>
+      <c r="F316" s="14"/>
+    </row>
+    <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A317" s="14"/>
+      <c r="B317" s="14"/>
+      <c r="C317" s="14"/>
+      <c r="D317" s="14"/>
+      <c r="E317" s="14"/>
+      <c r="F317" s="14"/>
+    </row>
+    <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A318" s="14"/>
+      <c r="B318" s="14"/>
+      <c r="C318" s="14"/>
+      <c r="D318" s="14"/>
+      <c r="E318" s="14"/>
+      <c r="F318" s="14"/>
+    </row>
+    <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A319" s="14"/>
+      <c r="B319" s="14"/>
+      <c r="C319" s="14"/>
+      <c r="D319" s="14"/>
+      <c r="E319" s="14"/>
+      <c r="F319" s="14"/>
+    </row>
+    <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A320" s="14"/>
+      <c r="B320" s="14"/>
+      <c r="C320" s="14"/>
+      <c r="D320" s="14"/>
+      <c r="E320" s="14"/>
+      <c r="F320" s="14"/>
+    </row>
+    <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A321" s="14"/>
+      <c r="B321" s="14"/>
+      <c r="C321" s="14"/>
+      <c r="D321" s="14"/>
+      <c r="E321" s="14"/>
+      <c r="F321" s="14"/>
+    </row>
+    <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A322" s="14"/>
+      <c r="B322" s="14"/>
+      <c r="C322" s="14"/>
+      <c r="D322" s="14"/>
+      <c r="E322" s="14"/>
+      <c r="F322" s="14"/>
+    </row>
+    <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A323" s="14"/>
+      <c r="B323" s="14"/>
+      <c r="C323" s="14"/>
+      <c r="D323" s="14"/>
+      <c r="E323" s="14"/>
+      <c r="F323" s="14"/>
+    </row>
+    <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A324" s="14"/>
+      <c r="B324" s="14"/>
+      <c r="C324" s="14"/>
+      <c r="D324" s="14"/>
+      <c r="E324" s="14"/>
+      <c r="F324" s="14"/>
+    </row>
+    <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A325" s="14"/>
+      <c r="B325" s="14"/>
+      <c r="C325" s="14"/>
+      <c r="D325" s="14"/>
+      <c r="E325" s="14"/>
+      <c r="F325" s="14"/>
+    </row>
+    <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A326" s="14"/>
+      <c r="B326" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C326" s="14"/>
+      <c r="D326" s="14"/>
+      <c r="E326" s="14"/>
+      <c r="F326" s="14"/>
+    </row>
+    <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A327" s="14"/>
+      <c r="B327" s="14"/>
+      <c r="C327" s="14"/>
+      <c r="D327" s="14"/>
+      <c r="E327" s="14"/>
+      <c r="F327" s="14"/>
+    </row>
+    <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A328" s="14"/>
+      <c r="B328" s="14"/>
+      <c r="C328" s="14"/>
+      <c r="D328" s="14"/>
+      <c r="E328" s="14"/>
+      <c r="F328" s="14"/>
+    </row>
+    <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A329" s="14"/>
+      <c r="B329" s="14"/>
+      <c r="C329" s="14"/>
+      <c r="D329" s="14"/>
+      <c r="E329" s="14"/>
+      <c r="F329" s="14"/>
+    </row>
+    <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A330" s="14"/>
+      <c r="B330" s="14"/>
+      <c r="C330" s="14"/>
+      <c r="D330" s="14"/>
+      <c r="E330" s="14"/>
+      <c r="F330" s="14"/>
+    </row>
+    <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A331" s="14"/>
+      <c r="B331" s="14"/>
+      <c r="C331" s="14"/>
+      <c r="D331" s="14"/>
+      <c r="E331" s="14"/>
+      <c r="F331" s="14"/>
+    </row>
+    <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A332" s="14"/>
+      <c r="B332" s="14"/>
+      <c r="C332" s="14"/>
+      <c r="D332" s="14"/>
+      <c r="E332" s="14"/>
+      <c r="F332" s="14"/>
+    </row>
+    <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A333" s="14"/>
+      <c r="B333" s="14"/>
+      <c r="C333" s="14"/>
+      <c r="D333" s="14"/>
+      <c r="E333" s="14"/>
+      <c r="F333" s="14"/>
+    </row>
+    <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A334" s="14"/>
+      <c r="B334" s="14"/>
+      <c r="C334" s="14"/>
+      <c r="D334" s="14"/>
+      <c r="E334" s="14"/>
+      <c r="F334" s="14"/>
+    </row>
+    <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A335" s="14"/>
+      <c r="B335" s="14"/>
+      <c r="C335" s="14"/>
+      <c r="D335" s="14"/>
+      <c r="E335" s="14"/>
+      <c r="F335" s="14"/>
+    </row>
+    <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A336" s="14"/>
+      <c r="B336" s="14"/>
+      <c r="C336" s="14"/>
+      <c r="D336" s="14"/>
+      <c r="E336" s="14"/>
+      <c r="F336" s="14"/>
+    </row>
+    <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A337" s="14"/>
+      <c r="B337" s="14"/>
+      <c r="C337" s="14"/>
+      <c r="D337" s="14"/>
+      <c r="E337" s="14"/>
+      <c r="F337" s="14"/>
+    </row>
+    <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A338" s="14"/>
+      <c r="B338" s="14"/>
+      <c r="C338" s="14"/>
+      <c r="D338" s="14"/>
+      <c r="E338" s="14"/>
+      <c r="F338" s="14"/>
+    </row>
+    <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A339" s="14"/>
+      <c r="B339" s="14"/>
+      <c r="C339" s="14"/>
+      <c r="D339" s="14"/>
+      <c r="E339" s="14"/>
+      <c r="F339" s="14"/>
+    </row>
+    <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A340" s="14"/>
+      <c r="B340" s="14"/>
+      <c r="C340" s="14"/>
+      <c r="D340" s="14"/>
+      <c r="E340" s="14"/>
+      <c r="F340" s="14"/>
+    </row>
+    <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A341" s="14"/>
+      <c r="B341" s="14"/>
+      <c r="C341" s="14"/>
+      <c r="D341" s="14"/>
+      <c r="E341" s="14"/>
+      <c r="F341" s="14"/>
+    </row>
+    <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A342" s="14"/>
+      <c r="B342" s="14"/>
+      <c r="C342" s="14"/>
+      <c r="D342" s="14"/>
+      <c r="E342" s="14"/>
+      <c r="F342" s="14"/>
+    </row>
+    <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A343" s="14"/>
+      <c r="B343" s="14"/>
+      <c r="C343" s="14"/>
+      <c r="D343" s="14"/>
+      <c r="E343" s="14"/>
+      <c r="F343" s="14"/>
+    </row>
+    <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A344" s="14"/>
+      <c r="B344" s="14"/>
+      <c r="C344" s="14"/>
+      <c r="D344" s="14"/>
+      <c r="E344" s="14"/>
+      <c r="F344" s="14"/>
+    </row>
+    <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A345" s="14"/>
+      <c r="B345" s="14"/>
+      <c r="C345" s="14"/>
+      <c r="D345" s="14"/>
+      <c r="E345" s="14"/>
+      <c r="F345" s="14"/>
+    </row>
+    <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A346" s="14"/>
+      <c r="B346" s="14"/>
+      <c r="C346" s="14"/>
+      <c r="D346" s="14"/>
+      <c r="E346" s="14"/>
+      <c r="F346" s="14"/>
+    </row>
+    <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A347" s="14"/>
+      <c r="B347" s="14"/>
+      <c r="C347" s="14"/>
+      <c r="D347" s="14"/>
+      <c r="E347" s="14"/>
+      <c r="F347" s="14"/>
+    </row>
+    <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A348" s="14"/>
+      <c r="B348" s="14"/>
+      <c r="C348" s="14"/>
+      <c r="D348" s="14"/>
+      <c r="E348" s="14"/>
+      <c r="F348" s="14"/>
+    </row>
+    <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A349" s="14"/>
+      <c r="B349" s="14"/>
+      <c r="C349" s="14"/>
+      <c r="D349" s="14"/>
+      <c r="E349" s="14"/>
+      <c r="F349" s="14"/>
+    </row>
+    <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A350" s="14"/>
+      <c r="B350" s="14"/>
+      <c r="C350" s="14"/>
+      <c r="D350" s="14"/>
+      <c r="E350" s="14"/>
+      <c r="F350" s="14"/>
+    </row>
+    <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A351" s="14"/>
+      <c r="B351" s="14"/>
+      <c r="C351" s="14"/>
+      <c r="D351" s="14"/>
+      <c r="E351" s="14"/>
+      <c r="F351" s="14"/>
+    </row>
+    <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A352" s="14"/>
+      <c r="B352" s="14"/>
+      <c r="C352" s="14"/>
+      <c r="D352" s="14"/>
+      <c r="E352" s="14"/>
+      <c r="F352" s="14"/>
+    </row>
+    <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A353" s="14"/>
+      <c r="B353" s="14"/>
+      <c r="C353" s="14"/>
+      <c r="D353" s="14"/>
+      <c r="E353" s="14"/>
+      <c r="F353" s="14"/>
+    </row>
+    <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A354" s="14"/>
+      <c r="B354" s="14"/>
+      <c r="C354" s="14"/>
+      <c r="D354" s="14"/>
+      <c r="E354" s="14"/>
+      <c r="F354" s="14"/>
+    </row>
+    <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A355" s="14"/>
+      <c r="B355" s="14"/>
+      <c r="C355" s="14"/>
+      <c r="D355" s="14"/>
+      <c r="E355" s="14"/>
+      <c r="F355" s="14"/>
+    </row>
+    <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A356" s="14"/>
+      <c r="B356" s="14"/>
+      <c r="C356" s="14"/>
+      <c r="D356" s="14"/>
+      <c r="E356" s="14"/>
+      <c r="F356" s="14"/>
+    </row>
+    <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A357" s="14"/>
+      <c r="B357" s="14"/>
+      <c r="C357" s="14"/>
+      <c r="D357" s="14"/>
+      <c r="E357" s="14"/>
+      <c r="F357" s="14"/>
+    </row>
+    <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A358" s="14"/>
+      <c r="B358" s="14"/>
+      <c r="C358" s="14"/>
+      <c r="D358" s="14"/>
+      <c r="E358" s="14"/>
+      <c r="F358" s="14"/>
+    </row>
+    <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A359" s="14"/>
+      <c r="B359" s="14"/>
+      <c r="C359" s="14"/>
+      <c r="D359" s="14"/>
+      <c r="E359" s="14"/>
+      <c r="F359" s="14"/>
+    </row>
+    <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A360" s="14"/>
+      <c r="B360" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C360" s="14"/>
+      <c r="D360" s="14"/>
+      <c r="E360" s="14"/>
+      <c r="F360" s="14"/>
+    </row>
+    <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A361" s="14"/>
+      <c r="B361" s="14"/>
+      <c r="C361" s="14"/>
+      <c r="D361" s="14"/>
+      <c r="E361" s="14"/>
+      <c r="F361" s="14"/>
+    </row>
+    <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A362" s="14"/>
+      <c r="B362" s="14"/>
+      <c r="C362" s="14"/>
+      <c r="D362" s="14"/>
+      <c r="E362" s="14"/>
+      <c r="F362" s="14"/>
+    </row>
+    <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A363" s="14"/>
+      <c r="B363" s="14"/>
+      <c r="C363" s="14"/>
+      <c r="D363" s="14"/>
+      <c r="E363" s="14"/>
+      <c r="F363" s="14"/>
+    </row>
+    <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A364" s="14"/>
+      <c r="B364" s="14"/>
+      <c r="C364" s="14"/>
+      <c r="D364" s="14"/>
+      <c r="E364" s="14"/>
+      <c r="F364" s="14"/>
+    </row>
+    <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A365" s="14"/>
+      <c r="B365" s="14"/>
+      <c r="C365" s="14"/>
+      <c r="D365" s="14"/>
+      <c r="E365" s="14"/>
+      <c r="F365" s="14"/>
+    </row>
+    <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A366" s="14"/>
+      <c r="B366" s="14"/>
+      <c r="C366" s="14"/>
+      <c r="D366" s="14"/>
+      <c r="E366" s="14"/>
+      <c r="F366" s="14"/>
+    </row>
+    <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A367" s="14"/>
+      <c r="B367" s="14"/>
+      <c r="C367" s="14"/>
+      <c r="D367" s="14"/>
+      <c r="E367" s="14"/>
+      <c r="F367" s="14"/>
+    </row>
+    <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A368" s="14"/>
+      <c r="B368" s="14"/>
+      <c r="C368" s="14"/>
+      <c r="D368" s="14"/>
+      <c r="E368" s="14"/>
+      <c r="F368" s="14"/>
+    </row>
+    <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A369" s="14"/>
+      <c r="B369" s="14"/>
+      <c r="C369" s="14"/>
+      <c r="D369" s="14"/>
+      <c r="E369" s="14"/>
+      <c r="F369" s="14"/>
+    </row>
+    <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A370" s="14"/>
+      <c r="B370" s="14"/>
+      <c r="C370" s="14"/>
+      <c r="D370" s="14"/>
+      <c r="E370" s="14"/>
+      <c r="F370" s="14"/>
+    </row>
+    <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A371" s="14"/>
+      <c r="B371" s="14"/>
+      <c r="C371" s="14"/>
+      <c r="D371" s="14"/>
+      <c r="E371" s="14"/>
+      <c r="F371" s="14"/>
+    </row>
+    <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A372" s="14"/>
+      <c r="B372" s="14"/>
+      <c r="C372" s="14"/>
+      <c r="D372" s="14"/>
+      <c r="E372" s="14"/>
+      <c r="F372" s="14"/>
+    </row>
+    <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A373" s="14"/>
+      <c r="B373" s="14"/>
+      <c r="C373" s="14"/>
+      <c r="D373" s="14"/>
+      <c r="E373" s="14"/>
+      <c r="F373" s="14"/>
+    </row>
+    <row r="374" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A374" s="14"/>
+      <c r="B374" s="14"/>
+      <c r="C374" s="14"/>
+      <c r="D374" s="14"/>
+      <c r="E374" s="14"/>
+      <c r="F374" s="14"/>
+    </row>
+    <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A375" s="14"/>
+      <c r="B375" s="14"/>
+      <c r="C375" s="14"/>
+      <c r="D375" s="14"/>
+      <c r="E375" s="14"/>
+      <c r="F375" s="14"/>
+    </row>
+    <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A376" s="14"/>
+      <c r="B376" s="14"/>
+      <c r="C376" s="14"/>
+      <c r="D376" s="14"/>
+      <c r="E376" s="14"/>
+      <c r="F376" s="14"/>
+    </row>
+    <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A377" s="14"/>
+      <c r="B377" s="14"/>
+      <c r="C377" s="14"/>
+      <c r="D377" s="14"/>
+      <c r="E377" s="14"/>
+      <c r="F377" s="14"/>
+    </row>
+    <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A378" s="14"/>
+      <c r="B378" s="14"/>
+      <c r="C378" s="14"/>
+      <c r="D378" s="14"/>
+      <c r="E378" s="14"/>
+      <c r="F378" s="14"/>
+    </row>
+    <row r="379" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A379" s="14"/>
+      <c r="B379" s="14"/>
+      <c r="C379" s="14"/>
+      <c r="D379" s="14"/>
+      <c r="E379" s="14"/>
+      <c r="F379" s="14"/>
+    </row>
+    <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A380" s="14"/>
+      <c r="B380" s="14"/>
+      <c r="C380" s="14"/>
+      <c r="D380" s="14"/>
+      <c r="E380" s="14"/>
+      <c r="F380" s="14"/>
+    </row>
+    <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A381" s="14"/>
+      <c r="B381" s="14"/>
+      <c r="C381" s="14"/>
+      <c r="D381" s="14"/>
+      <c r="E381" s="14"/>
+      <c r="F381" s="14"/>
+    </row>
+    <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A382" s="14"/>
+      <c r="B382" s="14"/>
+      <c r="C382" s="14"/>
+      <c r="D382" s="14"/>
+      <c r="E382" s="14"/>
+      <c r="F382" s="14"/>
+    </row>
+    <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A383" s="14"/>
+      <c r="B383" s="14"/>
+      <c r="C383" s="14"/>
+      <c r="D383" s="14"/>
+      <c r="E383" s="14"/>
+      <c r="F383" s="14"/>
+    </row>
+    <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A384" s="14"/>
+      <c r="B384" s="14"/>
+      <c r="C384" s="14"/>
+      <c r="D384" s="14"/>
+      <c r="E384" s="14"/>
+      <c r="F384" s="14"/>
+    </row>
+    <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A385" s="14"/>
+      <c r="B385" s="14"/>
+      <c r="C385" s="14"/>
+      <c r="D385" s="14"/>
+      <c r="E385" s="14"/>
+      <c r="F385" s="14"/>
+    </row>
+    <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A386" s="14"/>
+      <c r="B386" s="14"/>
+      <c r="C386" s="14"/>
+      <c r="D386" s="14"/>
+      <c r="E386" s="14"/>
+      <c r="F386" s="14"/>
+    </row>
+    <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A387" s="14"/>
+      <c r="B387" s="14"/>
+      <c r="C387" s="14"/>
+      <c r="D387" s="14"/>
+      <c r="E387" s="14"/>
+      <c r="F387" s="14"/>
+    </row>
+    <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A388" s="14"/>
+      <c r="B388" s="14"/>
+      <c r="C388" s="14"/>
+      <c r="D388" s="14"/>
+      <c r="E388" s="14"/>
+      <c r="F388" s="14"/>
+    </row>
+    <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A389" s="14"/>
+      <c r="B389" s="14"/>
+      <c r="C389" s="14"/>
+      <c r="D389" s="14"/>
+      <c r="E389" s="14"/>
+      <c r="F389" s="14"/>
+    </row>
+    <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A390" s="14"/>
+      <c r="B390" s="14"/>
+      <c r="C390" s="14"/>
+      <c r="D390" s="14"/>
+      <c r="E390" s="14"/>
+      <c r="F390" s="14"/>
+    </row>
+    <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A391" s="14"/>
+      <c r="B391" s="14"/>
+      <c r="C391" s="14"/>
+      <c r="D391" s="14"/>
+      <c r="E391" s="14"/>
+      <c r="F391" s="14"/>
+    </row>
+    <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A392" s="14"/>
+      <c r="B392" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C392" s="14"/>
+      <c r="D392" s="14"/>
+      <c r="E392" s="14"/>
+      <c r="F392" s="14"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>